<commit_message>
Final changes - 2nd June 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTT0046984_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheBuysideDeals_NeitherSubjectNorBuyerIsAPotentialRoundTrip.xlsx
+++ b/TestData/TMTT0046984_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheBuysideDeals_NeitherSubjectNorBuyerIsAPotentialRoundTrip.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CB2A65-04BE-4A84-A7CD-E5B8951400AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFBAFC3-6357-426F-AC6D-974738B57417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="568" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="568" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -295,9 +295,6 @@
     <t>Reason</t>
   </si>
   <si>
-    <t>Comment</t>
-  </si>
-  <si>
     <t>Change Company Type</t>
   </si>
   <si>
@@ -313,18 +310,9 @@
     <t>Warning Msg 2</t>
   </si>
   <si>
-    <t>Requesting to change Company Type to Operating Company and Ownership to Private Equity Group because it is being considered to be a potential round trip</t>
-  </si>
-  <si>
     <t>Warning Msg 3</t>
   </si>
   <si>
-    <t>Comment 2</t>
-  </si>
-  <si>
-    <t>Requesting to change Company Type to Operating Company with Ownership: Private Equity Group because it is being considered to be a potential round trip</t>
-  </si>
-  <si>
     <t>The Subject and Buyer in this engagement satisfy the requirements of a round trip. If this Subject or Buyer is worth pursuing as a round trip candidate, please change the value to "Subject is a Round Trip" or "Buyer is a round trip".</t>
   </si>
   <si>
@@ -350,6 +338,18 @@
   </si>
   <si>
     <t>Caledonia Investments Plc</t>
+  </si>
+  <si>
+    <t>The Subject in this engagement satisfies the requirements of a round trip. Please confirm with the deal team or CF operations team.</t>
+  </si>
+  <si>
+    <t>Subject Comment</t>
+  </si>
+  <si>
+    <t>Client Comment</t>
+  </si>
+  <si>
+    <t>The Buyer in this engagement satisfies the requirements of a round trip. Please confirm with the deal team or CF operations team.</t>
   </si>
 </sst>
 </file>
@@ -726,7 +726,7 @@
         <v>65</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -734,7 +734,7 @@
         <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -871,21 +871,21 @@
         <v>81</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>88</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -903,7 +903,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1175537-D85E-4D33-8AD2-B3C163BE409D}">
   <dimension ref="A1:AD5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
@@ -1012,10 +1012,10 @@
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C2" t="s">
         <v>37</v>
@@ -1104,10 +1104,10 @@
     </row>
     <row r="3" spans="1:30" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C3" t="s">
         <v>37</v>
@@ -1196,10 +1196,10 @@
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C4" t="s">
         <v>37</v>
@@ -1247,7 +1247,7 @@
         <v>75</v>
       </c>
       <c r="R4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="S4" t="s">
         <v>74</v>
@@ -1288,10 +1288,10 @@
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s">
         <v>37</v>
@@ -1339,7 +1339,7 @@
         <v>75</v>
       </c>
       <c r="R5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="S5" t="s">
         <v>74</v>
@@ -1529,8 +1529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92EA0090-8A70-4EE9-9BBD-D73C51089E4F}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1544,21 +1544,21 @@
         <v>82</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FInal - 13 June 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTT0046984_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheBuysideDeals_NeitherSubjectNorBuyerIsAPotentialRoundTrip.xlsx
+++ b/TestData/TMTT0046984_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheBuysideDeals_NeitherSubjectNorBuyerIsAPotentialRoundTrip.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFBAFC3-6357-426F-AC6D-974738B57417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A16458-E162-4F82-B886-D7D12A1E085A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="568" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="568" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="101">
   <si>
     <t>Subject</t>
   </si>
@@ -311,9 +311,6 @@
   </si>
   <si>
     <t>Warning Msg 3</t>
-  </si>
-  <si>
-    <t>The Subject and Buyer in this engagement satisfy the requirements of a round trip. If this Subject or Buyer is worth pursuing as a round trip candidate, please change the value to "Subject is a Round Trip" or "Buyer is a round trip".</t>
   </si>
   <si>
     <t>ICU Medical, Inc.</t>
@@ -856,7 +853,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -879,13 +876,13 @@
     </row>
     <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1012,10 +1009,10 @@
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" t="s">
         <v>90</v>
-      </c>
-      <c r="B2" t="s">
-        <v>91</v>
       </c>
       <c r="C2" t="s">
         <v>37</v>
@@ -1104,10 +1101,10 @@
     </row>
     <row r="3" spans="1:30" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C3" t="s">
         <v>37</v>
@@ -1196,10 +1193,10 @@
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
         <v>37</v>
@@ -1288,10 +1285,10 @@
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" t="s">
         <v>90</v>
-      </c>
-      <c r="B5" t="s">
-        <v>91</v>
       </c>
       <c r="C5" t="s">
         <v>37</v>
@@ -1387,8 +1384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C30D5517-1C18-480A-9228-B12CD8B6EC9B}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1417,7 +1414,7 @@
         <v>77</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1428,7 +1425,7 @@
         <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1439,7 +1436,7 @@
         <v>77</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1450,7 +1447,7 @@
         <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1529,7 +1526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92EA0090-8A70-4EE9-9BBD-D73C51089E4F}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -1544,10 +1541,10 @@
         <v>82</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>99</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -1555,10 +1552,10 @@
         <v>83</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Engagement round trip changes - mid - 23 June 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTT0046984_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheBuysideDeals_NeitherSubjectNorBuyerIsAPotentialRoundTrip.xlsx
+++ b/TestData/TMTT0046984_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheBuysideDeals_NeitherSubjectNorBuyerIsAPotentialRoundTrip.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A16458-E162-4F82-B886-D7D12A1E085A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03BE2B9B-05F7-4F53-9357-B6CCDC28CB71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="568" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="568" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="101">
   <si>
     <t>Subject</t>
   </si>
@@ -898,10 +898,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1175537-D85E-4D33-8AD2-B3C163BE409D}">
-  <dimension ref="A1:AD5"/>
+  <dimension ref="A1:AD4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1283,98 +1283,6 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" t="s">
-        <v>40</v>
-      </c>
-      <c r="I5" t="s">
-        <v>39</v>
-      </c>
-      <c r="J5" t="s">
-        <v>39</v>
-      </c>
-      <c r="K5" t="s">
-        <v>41</v>
-      </c>
-      <c r="L5" t="s">
-        <v>42</v>
-      </c>
-      <c r="M5" t="s">
-        <v>43</v>
-      </c>
-      <c r="N5" t="s">
-        <v>66</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="R5" t="s">
-        <v>86</v>
-      </c>
-      <c r="S5" t="s">
-        <v>74</v>
-      </c>
-      <c r="T5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="U5" t="s">
-        <v>45</v>
-      </c>
-      <c r="V5" t="s">
-        <v>46</v>
-      </c>
-      <c r="W5" t="s">
-        <v>47</v>
-      </c>
-      <c r="X5" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA5" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="AB5" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>66</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>51</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1384,7 +1292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C30D5517-1C18-480A-9228-B12CD8B6EC9B}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>